<commit_message>
Added description and data driven for login
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Data.xlsx
+++ b/src/main/resources/data/Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CarRentalProject\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pooja_shitole\Workspace1\CarRental\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029F2592-2F18-462D-8A83-0E466BB02125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14051F61-2466-4332-84BC-BBF77063A6E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -58,6 +59,18 @@
   </si>
   <si>
     <t>emma123</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@12345</t>
   </si>
 </sst>
 </file>
@@ -388,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,4 +471,43 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443799CA-FA04-48E6-A668-714F17EC0314}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9F28E54F-0556-49F0-9D0E-90DFABACA859}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{335D9478-20DD-406C-9792-C18F7AD5E8F3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
selenium Grid script added
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Data.xlsx
+++ b/src/main/resources/data/Data.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pooja_shitole\Workspace1\CarRental\src\main\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14051F61-2466-4332-84BC-BBF77063A6E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2143D205-4811-4750-AF72-2B9458FC8662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14440" windowHeight="10780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -401,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -477,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443799CA-FA04-48E6-A668-714F17EC0314}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>